<commit_message>
EUR ITALY: add 3 new bond
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/EUR/EUR_ITALY.xlsx
+++ b/QuantLibXL/Data2/XLS/EUR/EUR_ITALY.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1136" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1139" uniqueCount="457">
   <si>
     <t>General Settings</t>
   </si>
@@ -1410,6 +1410,15 @@
   </si>
   <si>
     <t>IT0005069395</t>
+  </si>
+  <si>
+    <t>IT0005083057</t>
+  </si>
+  <si>
+    <t>IT0005090318</t>
+  </si>
+  <si>
+    <t>IT0005086886</t>
   </si>
 </sst>
 </file>
@@ -1417,7 +1426,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="11">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
@@ -1845,7 +1854,7 @@
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="140">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="4" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
@@ -2063,10 +2072,8 @@
     <xf numFmtId="169" fontId="9" fillId="0" borderId="22" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="9" fillId="0" borderId="22" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="9" fillId="0" borderId="22" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="16" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2476,17 +2483,17 @@
     <row r="1" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="str">
         <f>_xll.qlxlVersion(TRUE,Trigger)</f>
-        <v>QuantLibXL 1.5.0 - MS VC++ 9.0 - Multithreaded Dynamic Runtime library - Release Configuration - Nov 18 2014 09:26:00</v>
+        <v>QuantLibXL 1.5.0 - MS VC++ 9.0 - Multithreaded Dynamic Runtime library - Release Configuration - Dec 24 2014 09:17:06</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
-      <c r="B2" s="137" t="s">
+      <c r="B2" s="135" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="138"/>
-      <c r="D2" s="138"/>
-      <c r="E2" s="139"/>
+      <c r="C2" s="136"/>
+      <c r="D2" s="136"/>
+      <c r="E2" s="137"/>
     </row>
     <row r="3" spans="1:5" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
@@ -2502,7 +2509,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="9">
-        <v>41929.461469907408</v>
+        <v>42065.649004629631</v>
       </c>
       <c r="E4" s="10"/>
     </row>
@@ -3189,9 +3196,9 @@
         <f>_xll.qlSchedule(C8&amp;"_Sch",D8,E8,F8,G8,H8,I8,J8,K8,L8,M8,Permanent,Trigger,ObjectOverwrite)</f>
         <v>IT0003605380_Sch#0000</v>
       </c>
-      <c r="AD8" s="51" t="e">
+      <c r="AD8" s="51" t="str">
         <f>IF(AE8,_xll.qlCCTEU(C8,,E8,X8,W8,D8,,Permanent,Trigger,ObjectOverwrite),_xll.qlFloatingRateBond(C8,AB8,N8,O8,P8,Q8,AC8,R8,S8,T8,U8,V8,W8,X8,Y8,Z8,AA8,Permanent,Trigger,ObjectOverwrite))</f>
-        <v>#NUM!</v>
+        <v>IT0003605380#0000</v>
       </c>
       <c r="AE8" s="51" t="b">
         <v>0</v>
@@ -3283,9 +3290,9 @@
         <f>_xll.qlSchedule(C9&amp;"_Sch",D9,E9,F9,G9,H9,I9,J9,K9,L9,M9,Permanent,Trigger,ObjectOverwrite)</f>
         <v>IT0003658009_Sch#0000</v>
       </c>
-      <c r="AD9" s="51" t="e">
+      <c r="AD9" s="51" t="str">
         <f>IF(AE9,_xll.qlCCTEU(C9,,E9,X9,W9,D9,,Permanent,Trigger,ObjectOverwrite),_xll.qlFloatingRateBond(C9,AB9,N9,O9,P9,Q9,AC9,R9,S9,T9,U9,V9,W9,X9,Y9,Z9,AA9,Permanent,Trigger,ObjectOverwrite))</f>
-        <v>#NUM!</v>
+        <v>IT0003658009#0000</v>
       </c>
       <c r="AE9" s="51" t="b">
         <v>0</v>
@@ -3377,9 +3384,9 @@
         <f>_xll.qlSchedule(C10&amp;"_Sch",D10,E10,F10,G10,H10,I10,J10,K10,L10,M10,Permanent,Trigger,ObjectOverwrite)</f>
         <v>IT0003746366_Sch#0000</v>
       </c>
-      <c r="AD10" s="51" t="e">
+      <c r="AD10" s="51" t="str">
         <f>IF(AE10,_xll.qlCCTEU(C10,,E10,X10,W10,D10,,Permanent,Trigger,ObjectOverwrite),_xll.qlFloatingRateBond(C10,AB10,N10,O10,P10,Q10,AC10,R10,S10,T10,U10,V10,W10,X10,Y10,Z10,AA10,Permanent,Trigger,ObjectOverwrite))</f>
-        <v>#NUM!</v>
+        <v>IT0003746366#0000</v>
       </c>
       <c r="AE10" s="51" t="b">
         <v>0</v>
@@ -3471,9 +3478,9 @@
         <f>_xll.qlSchedule(C11&amp;"_Sch",D11,E11,F11,G11,H11,I11,J11,K11,L11,M11,Permanent,Trigger,ObjectOverwrite)</f>
         <v>IT0003858856_Sch#0000</v>
       </c>
-      <c r="AD11" s="31" t="e">
+      <c r="AD11" s="31" t="str">
         <f>IF(AE11,_xll.qlCCTEU(C11,,E11,X11,W11,D11,,Permanent,Trigger,ObjectOverwrite),_xll.qlFloatingRateBond(C11,AB11,N11,O11,P11,Q11,AC11,R11,S11,T11,U11,V11,W11,X11,Y11,Z11,AA11,Permanent,Trigger,ObjectOverwrite))</f>
-        <v>#NUM!</v>
+        <v>IT0003858856#0000</v>
       </c>
       <c r="AE11" s="31" t="b">
         <v>0</v>
@@ -3565,9 +3572,9 @@
         <f>_xll.qlSchedule(C12&amp;"_Sch",D12,E12,F12,G12,H12,I12,J12,K12,L12,M12,Permanent,Trigger,ObjectOverwrite)</f>
         <v>IT0003993158_Sch#0000</v>
       </c>
-      <c r="AD12" s="31" t="e">
+      <c r="AD12" s="31" t="str">
         <f>IF(AE12,_xll.qlCCTEU(C12,,E12,X12,W12,D12,,Permanent,Trigger,ObjectOverwrite),_xll.qlFloatingRateBond(C12,AB12,N12,O12,P12,Q12,AC12,R12,S12,T12,U12,V12,W12,X12,Y12,Z12,AA12,Permanent,Trigger,ObjectOverwrite))</f>
-        <v>#NUM!</v>
+        <v>IT0003993158#0000</v>
       </c>
       <c r="AE12" s="31" t="b">
         <v>0</v>
@@ -3659,9 +3666,9 @@
         <f>_xll.qlSchedule(C13&amp;"_Sch",D13,E13,F13,G13,H13,I13,J13,K13,L13,M13,Permanent,Trigger,ObjectOverwrite)</f>
         <v>IT0004101447_Sch#0000</v>
       </c>
-      <c r="AD13" s="31" t="e">
+      <c r="AD13" s="31" t="str">
         <f>IF(AE13,_xll.qlCCTEU(C13,,E13,X13,W13,D13,,Permanent,Trigger,ObjectOverwrite),_xll.qlFloatingRateBond(C13,AB13,N13,O13,P13,Q13,AC13,R13,S13,T13,U13,V13,W13,X13,Y13,Z13,AA13,Permanent,Trigger,ObjectOverwrite))</f>
-        <v>#NUM!</v>
+        <v>IT0004101447#0000</v>
       </c>
       <c r="AE13" s="31" t="b">
         <v>0</v>
@@ -3753,9 +3760,9 @@
         <f>_xll.qlSchedule(C14&amp;"_Sch",D14,E14,F14,G14,H14,I14,J14,K14,L14,M14,Permanent,Trigger,ObjectOverwrite)</f>
         <v>IT0004224041_Sch#0000</v>
       </c>
-      <c r="AD14" s="31" t="e">
+      <c r="AD14" s="31" t="str">
         <f>IF(AE14,_xll.qlCCTEU(C14,,E14,X14,W14,D14,,Permanent,Trigger,ObjectOverwrite),_xll.qlFloatingRateBond(C14,AB14,N14,O14,P14,Q14,AC14,R14,S14,T14,U14,V14,W14,X14,Y14,Z14,AA14,Permanent,Trigger,ObjectOverwrite))</f>
-        <v>#NUM!</v>
+        <v>IT0004224041#0000</v>
       </c>
       <c r="AE14" s="31" t="b">
         <v>0</v>
@@ -3847,9 +3854,9 @@
         <f>_xll.qlSchedule(C15&amp;"_Sch",D15,E15,F15,G15,H15,I15,J15,K15,L15,M15,Permanent,Trigger,ObjectOverwrite)</f>
         <v>IT0004321813_Sch#0000</v>
       </c>
-      <c r="AD15" s="31" t="e">
+      <c r="AD15" s="31" t="str">
         <f>IF(AE15,_xll.qlCCTEU(C15,,E15,X15,W15,D15,,Permanent,Trigger,ObjectOverwrite),_xll.qlFloatingRateBond(C15,AB15,N15,O15,P15,Q15,AC15,R15,S15,T15,U15,V15,W15,X15,Y15,Z15,AA15,Permanent,Trigger,ObjectOverwrite))</f>
-        <v>#NUM!</v>
+        <v>IT0004321813#0000</v>
       </c>
       <c r="AE15" s="31" t="b">
         <v>0</v>
@@ -3941,9 +3948,9 @@
         <f>_xll.qlSchedule(C16&amp;"_Sch",D16,E16,F16,G16,H16,I16,J16,K16,L16,M16,Permanent,Trigger,ObjectOverwrite)</f>
         <v>IT0004404965_Sch#0000</v>
       </c>
-      <c r="AD16" s="31" t="e">
+      <c r="AD16" s="31" t="str">
         <f>IF(AE16,_xll.qlCCTEU(C16,,E16,X16,W16,D16,,Permanent,Trigger,ObjectOverwrite),_xll.qlFloatingRateBond(C16,AB16,N16,O16,P16,Q16,AC16,R16,S16,T16,U16,V16,W16,X16,Y16,Z16,AA16,Permanent,Trigger,ObjectOverwrite))</f>
-        <v>#NUM!</v>
+        <v>IT0004404965#0000</v>
       </c>
       <c r="AE16" s="31" t="b">
         <v>0</v>
@@ -4128,9 +4135,9 @@
         <f>_xll.qlSchedule(C18&amp;"_Sch",D18,E18,F18,G18,H18,I18,J18,K18,L18,M18,Permanent,Trigger,ObjectOverwrite)</f>
         <v>IT0004518715_Sch#0000</v>
       </c>
-      <c r="AD18" s="31" t="e">
+      <c r="AD18" s="31" t="str">
         <f>IF(AE18,_xll.qlCCTEU(C18,,E18,X18,W18,D18,,Permanent,Trigger,ObjectOverwrite),_xll.qlFloatingRateBond(C18,AB18,N18,O18,P18,Q18,AC18,R18,S18,T18,U18,V18,W18,X18,Y18,Z18,AA18,Permanent,Trigger,ObjectOverwrite))</f>
-        <v>#NUM!</v>
+        <v>IT0004518715#0000</v>
       </c>
       <c r="AE18" s="31" t="b">
         <v>0</v>
@@ -4222,9 +4229,9 @@
         <f>_xll.qlSchedule(C19&amp;"_Sch",D19,E19,F19,G19,H19,I19,J19,K19,L19,M19,Permanent,Trigger,ObjectOverwrite)</f>
         <v>IT0004584204_Sch#0000</v>
       </c>
-      <c r="AD19" s="31" t="e">
+      <c r="AD19" s="31" t="str">
         <f>IF(AE19,_xll.qlCCTEU(C19,,E19,X19,W19,D19,,Permanent,Trigger,ObjectOverwrite),_xll.qlFloatingRateBond(C19,AB19,N19,O19,P19,Q19,AC19,R19,S19,T19,U19,V19,W19,X19,Y19,Z19,AA19,Permanent,Trigger,ObjectOverwrite))</f>
-        <v>#NUM!</v>
+        <v>IT0004584204#0000</v>
       </c>
       <c r="AE19" s="31" t="b">
         <v>0</v>
@@ -4524,13 +4531,13 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:R97"/>
+  <dimension ref="A1:R100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="8" ySplit="7" topLeftCell="I32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="7" topLeftCell="I29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -4614,7 +4621,7 @@
     <row r="4" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="62"/>
       <c r="B4" s="21" t="str">
-        <f>IF(Serialize,_xll.ohObjectSave(I8:I97,SerializationPath&amp;FileName,FileOverwrite,Serialize),"---")</f>
+        <f>IF(Serialize,_xll.ohObjectSave(I8:I100,SerializationPath&amp;FileName,FileOverwrite,Serialize),"---")</f>
         <v>---</v>
       </c>
       <c r="C4" s="25" t="s">
@@ -4662,7 +4669,7 @@
       <c r="H6" s="22"/>
       <c r="I6" s="50">
         <f>_xll.qlBondSettlementDate(I8,)</f>
-        <v>42018</v>
+        <v>42067</v>
       </c>
       <c r="J6" s="22"/>
       <c r="K6" s="22"/>
@@ -4734,7 +4741,7 @@
       </c>
       <c r="I8" s="88" t="str">
         <f>_xll.qlBTP2(C8,,D8,E8,F8,G8,H8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0003799597#0001</v>
+        <v>IT0003799597#0003</v>
       </c>
       <c r="J8" s="123" t="b">
         <v>0</v>
@@ -4782,13 +4789,13 @@
       </c>
       <c r="I9" s="88" t="str">
         <f>_xll.qlBTP2(C9,,D9,E9,F9,G9,H9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004196918#0001</v>
+        <v>IT0004196918#0003</v>
       </c>
       <c r="J9" s="123" t="b">
         <v>0</v>
       </c>
       <c r="K9" s="121" t="str">
-        <f t="shared" ref="K9:K76" si="0">IF(AND(J9,ISNA(L9),ISNA(M9)),"Residual Missing","--")</f>
+        <f t="shared" ref="K9:K77" si="0">IF(AND(J9,ISNA(L9),ISNA(M9)),"Residual Missing","--")</f>
         <v>--</v>
       </c>
       <c r="L9" s="48" t="e">
@@ -4827,7 +4834,7 @@
       </c>
       <c r="I10" s="88" t="str">
         <f>_xll.qlBTP2(C10,,D10,E10,F10,G10,H10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0003872923#0001</v>
+        <v>IT0003872923#0003</v>
       </c>
       <c r="J10" s="123" t="b">
         <v>0</v>
@@ -4872,7 +4879,7 @@
       </c>
       <c r="I11" s="88" t="str">
         <f>_xll.qlBTP2(C11,,D11,E11,F11,G11,H11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004254352#0001</v>
+        <v>IT0004254352#0003</v>
       </c>
       <c r="J11" s="123" t="b">
         <v>0</v>
@@ -4917,7 +4924,7 @@
       </c>
       <c r="I12" s="88" t="str">
         <f>_xll.qlBTP2(C12,,D12,E12,F12,G12,H12,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0001448619#0001</v>
+        <v>IT0001448619#0003</v>
       </c>
       <c r="J12" s="123" t="b">
         <v>1</v>
@@ -4965,7 +4972,7 @@
       </c>
       <c r="I13" s="88" t="str">
         <f>_xll.qlBTP2(C13,,D13,E13,F13,G13,H13,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004332521#0001</v>
+        <v>IT0004332521#0003</v>
       </c>
       <c r="J13" s="123" t="b">
         <v>0</v>
@@ -5010,7 +5017,7 @@
       </c>
       <c r="I14" s="88" t="str">
         <f>_xll.qlBTP2(C14,,D14,E14,F14,G14,H14,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004026297#0001</v>
+        <v>IT0004026297#0003</v>
       </c>
       <c r="J14" s="123" t="b">
         <v>0</v>
@@ -5055,7 +5062,7 @@
       </c>
       <c r="I15" s="88" t="str">
         <f>_xll.qlBTP2(C15,,D15,E15,F15,G15,H15,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0003080402#0001</v>
+        <v>IT0003080402#0003</v>
       </c>
       <c r="J15" s="123" t="b">
         <v>1</v>
@@ -5100,7 +5107,7 @@
       </c>
       <c r="I16" s="88" t="str">
         <f>_xll.qlBTP2(C16,,D16,E16,F16,G16,H16,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004404973#0001</v>
+        <v>IT0004404973#0003</v>
       </c>
       <c r="J16" s="123" t="b">
         <v>0</v>
@@ -5145,7 +5152,7 @@
       </c>
       <c r="I17" s="88" t="str">
         <f>_xll.qlBTP2(C17,,D17,E17,F17,G17,H17,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004112816#0001</v>
+        <v>IT0004112816#0003</v>
       </c>
       <c r="J17" s="123" t="b">
         <v>0</v>
@@ -5190,7 +5197,7 @@
       </c>
       <c r="I18" s="88" t="str">
         <f>_xll.qlBTP2(C18,,D18,E18,F18,G18,H18,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0003190912#0001</v>
+        <v>IT0003190912#0003</v>
       </c>
       <c r="J18" s="123" t="b">
         <v>1</v>
@@ -5235,10 +5242,10 @@
       </c>
       <c r="I19" s="88" t="str">
         <f>_xll.qlBTP2(C19,,D19,E19,F19,G19,H19,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004467483#0001</v>
+        <v>IT0004467483#0003</v>
       </c>
       <c r="J19" s="123" t="b">
-        <f t="shared" ref="J19:J90" si="1">NOT(ISNA(VLOOKUP(LEFT($I19,12),LatestStrippable,1,FALSE)))</f>
+        <f t="shared" ref="J19:J92" si="1">NOT(ISNA(VLOOKUP(LEFT($I19,12),LatestStrippable,1,FALSE)))</f>
         <v>0</v>
       </c>
       <c r="K19" s="121" t="str">
@@ -5249,7 +5256,7 @@
         <f>LEFT(VLOOKUP($D19,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
         <v>#N/A</v>
       </c>
-      <c r="M19" s="135" t="e">
+      <c r="M19" s="134" t="e">
         <f>LEFT(VLOOKUP($D19,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
         <v>#N/A</v>
       </c>
@@ -5281,7 +5288,7 @@
       </c>
       <c r="I20" s="88" t="str">
         <f>_xll.qlBTP2(C20,,D20,E20,F20,G20,H20,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004220627#0001</v>
+        <v>IT0004220627#0003</v>
       </c>
       <c r="J20" s="123" t="b">
         <f t="shared" si="1"/>
@@ -5295,7 +5302,7 @@
         <f>LEFT(VLOOKUP($D20,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
         <v>#N/A</v>
       </c>
-      <c r="M20" s="135" t="e">
+      <c r="M20" s="134" t="e">
         <f>LEFT(VLOOKUP($D20,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
         <v>#N/A</v>
       </c>
@@ -5327,7 +5334,7 @@
       </c>
       <c r="I21" s="88" t="str">
         <f>_xll.qlBTP2(C21,,D21,E21,F21,G21,H21,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004508971#0001</v>
+        <v>IT0004508971#0003</v>
       </c>
       <c r="J21" s="123" t="b">
         <f t="shared" si="1"/>
@@ -5373,7 +5380,7 @@
       </c>
       <c r="I22" s="88" t="str">
         <f>_xll.qlBTP2(C22,,D22,E22,F22,G22,H22,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004284334#0001</v>
+        <v>IT0004284334#0003</v>
       </c>
       <c r="J22" s="123" t="b">
         <f t="shared" si="1"/>
@@ -5419,7 +5426,7 @@
       </c>
       <c r="I23" s="88" t="str">
         <f>_xll.qlBTP2(C23,,D23,E23,F23,G23,H23,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004564636#0001</v>
+        <v>IT0004564636#0003</v>
       </c>
       <c r="J23" s="123" t="b">
         <f t="shared" si="1"/>
@@ -5465,7 +5472,7 @@
       </c>
       <c r="I24" s="88" t="str">
         <f>_xll.qlBTP2(C24,,D24,E24,F24,G24,H24,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0003357982#0001</v>
+        <v>IT0003357982#0003</v>
       </c>
       <c r="J24" s="123" t="b">
         <f t="shared" si="1"/>
@@ -5511,7 +5518,7 @@
       </c>
       <c r="I25" s="88" t="str">
         <f>_xll.qlBTP2(C25,,D25,E25,F25,G25,H25,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004365554#0001</v>
+        <v>IT0004365554#0003</v>
       </c>
       <c r="J25" s="123" t="b">
         <f t="shared" si="1"/>
@@ -5557,7 +5564,7 @@
       </c>
       <c r="I26" s="88" t="str">
         <f>_xll.qlBTP2(C26,,D26,E26,F26,G26,H26,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004612179#0001</v>
+        <v>IT0004612179#0003</v>
       </c>
       <c r="J26" s="125" t="b">
         <f t="shared" si="1"/>
@@ -5603,7 +5610,7 @@
       </c>
       <c r="I27" s="88" t="str">
         <f>_xll.qlBTP2(C27,,D27,E27,F27,G27,H27,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0003472336#0001</v>
+        <v>IT0003472336#0003</v>
       </c>
       <c r="J27" s="125" t="b">
         <f t="shared" si="1"/>
@@ -5649,7 +5656,7 @@
       </c>
       <c r="I28" s="88" t="str">
         <f>_xll.qlBTP2(C28,,D28,E28,F28,G28,H28,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004653108#0001</v>
+        <v>IT0004653108#0003</v>
       </c>
       <c r="J28" s="125" t="b">
         <f t="shared" si="1"/>
@@ -5695,7 +5702,7 @@
       </c>
       <c r="I29" s="88" t="str">
         <f>_xll.qlBTP2(C29,,D29,E29,F29,G29,H29,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004448863#0001</v>
+        <v>IT0004448863#0003</v>
       </c>
       <c r="J29" s="125" t="b">
         <f t="shared" si="1"/>
@@ -5741,7 +5748,7 @@
       </c>
       <c r="I30" s="116" t="str">
         <f>_xll.qlBTP2(C30,,D30,E30,F30,G30,H30,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004707995#0001</v>
+        <v>IT0004707995#0003</v>
       </c>
       <c r="J30" s="125" t="b">
         <f t="shared" si="1"/>
@@ -5787,7 +5794,7 @@
       </c>
       <c r="I31" s="116" t="str">
         <f>_xll.qlBTP2(C31,,D31,E31,F31,G31,H31,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004505076#0001</v>
+        <v>IT0004505076#0003</v>
       </c>
       <c r="J31" s="125" t="b">
         <f t="shared" si="1"/>
@@ -5833,7 +5840,7 @@
       </c>
       <c r="I32" s="116" t="str">
         <f>_xll.qlBTP2(C32,,D32,E32,F32,G32,H32,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004750409#0001</v>
+        <v>IT0004750409#0003</v>
       </c>
       <c r="J32" s="125" t="b">
         <f t="shared" si="1"/>
@@ -5879,7 +5886,7 @@
       </c>
       <c r="I33" s="116" t="str">
         <f>_xll.qlBTP2(C33,,D33,E33,F33,G33,H33,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0003618383#0001</v>
+        <v>IT0003618383#0003</v>
       </c>
       <c r="J33" s="125" t="b">
         <f t="shared" si="1"/>
@@ -5925,7 +5932,7 @@
       </c>
       <c r="I34" s="116" t="str">
         <f>_xll.qlBTP2(C34,,D34,E34,F34,G34,H34,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004780380#0001</v>
+        <v>IT0004780380#0003</v>
       </c>
       <c r="J34" s="125" t="b">
         <f t="shared" si="1"/>
@@ -5947,33 +5954,33 @@
     </row>
     <row r="35" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="19"/>
-      <c r="B35" s="126" t="str">
+      <c r="B35" s="124" t="str">
         <f>_xll.ohRangeRetrieveError(I35)</f>
         <v/>
       </c>
-      <c r="C35" s="40" t="s">
+      <c r="C35" s="112" t="s">
         <v>39</v>
       </c>
-      <c r="D35" s="85">
+      <c r="D35" s="113">
         <v>42036</v>
       </c>
-      <c r="E35" s="86">
+      <c r="E35" s="114">
         <v>4.2500000000000003E-2</v>
       </c>
-      <c r="F35" s="87">
-        <v>100</v>
-      </c>
-      <c r="G35" s="85">
+      <c r="F35" s="115">
+        <v>100</v>
+      </c>
+      <c r="G35" s="113">
         <v>38200</v>
       </c>
-      <c r="H35" s="85">
+      <c r="H35" s="113">
         <v>38231</v>
       </c>
-      <c r="I35" s="119" t="str">
+      <c r="I35" s="116" t="str">
         <f>_xll.qlBTP2(C35,,D35,E35,F35,G35,H35,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0003719918#0001</v>
-      </c>
-      <c r="J35" s="127" t="b">
+        <v>IT0003719918#0003</v>
+      </c>
+      <c r="J35" s="125" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -5993,33 +6000,33 @@
     </row>
     <row r="36" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="19"/>
-      <c r="B36" s="126" t="str">
+      <c r="B36" s="124" t="str">
         <f>_xll.ohRangeRetrieveError(I36)</f>
         <v/>
       </c>
-      <c r="C36" s="40" t="s">
+      <c r="C36" s="112" t="s">
         <v>429</v>
       </c>
-      <c r="D36" s="85">
+      <c r="D36" s="113">
         <v>42064</v>
       </c>
-      <c r="E36" s="86">
+      <c r="E36" s="114">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F36" s="87">
-        <v>100</v>
-      </c>
-      <c r="G36" s="85">
+      <c r="F36" s="115">
+        <v>100</v>
+      </c>
+      <c r="G36" s="113">
         <v>40969</v>
       </c>
-      <c r="H36" s="85">
+      <c r="H36" s="113">
         <v>40984</v>
       </c>
-      <c r="I36" s="119" t="str">
+      <c r="I36" s="116" t="str">
         <f>_xll.qlBTP2(C36,,D36,E36,F36,G36,H36,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004805070#0001</v>
-      </c>
-      <c r="J36" s="127" t="b">
+        <v>IT0004805070#0003</v>
+      </c>
+      <c r="J36" s="125" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -6063,7 +6070,7 @@
       </c>
       <c r="I37" s="119" t="str">
         <f>_xll.qlBTP2(C37,,D37,E37,F37,G37,H37,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004568272#0001</v>
+        <v>IT0004568272#0003</v>
       </c>
       <c r="J37" s="127" t="b">
         <f t="shared" si="1"/>
@@ -6109,7 +6116,7 @@
       </c>
       <c r="I38" s="119" t="str">
         <f>_xll.qlBTP2(C38,,D38,E38,F38,G38,H38,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004615917#0001</v>
+        <v>IT0004615917#0003</v>
       </c>
       <c r="J38" s="127" t="b">
         <f t="shared" si="1"/>
@@ -6155,7 +6162,7 @@
       </c>
       <c r="I39" s="119" t="str">
         <f>_xll.qlBTP2(C39,,D39,E39,F39,G39,H39,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004840788#0001</v>
+        <v>IT0004840788#0003</v>
       </c>
       <c r="J39" s="127" t="b">
         <f t="shared" si="1"/>
@@ -6201,7 +6208,7 @@
       </c>
       <c r="I40" s="119" t="str">
         <f>_xll.qlBTP2(C40,,D40,E40,F40,G40,H40,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0003844534#0001</v>
+        <v>IT0003844534#0003</v>
       </c>
       <c r="J40" s="127" t="b">
         <f t="shared" si="1"/>
@@ -6247,7 +6254,7 @@
       </c>
       <c r="I41" s="119" t="str">
         <f>_xll.qlBTP2(C41,,D41,E41,F41,G41,H41,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004656275#0001</v>
+        <v>IT0004656275#0003</v>
       </c>
       <c r="J41" s="127" t="b">
         <v>1</v>
@@ -6292,7 +6299,7 @@
       </c>
       <c r="I42" s="119" t="str">
         <f>_xll.qlBTP2(C42,,D42,E42,F42,G42,H42,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004880990#0001</v>
+        <v>IT0004880990#0003</v>
       </c>
       <c r="J42" s="127" t="b">
         <f t="shared" si="1"/>
@@ -6338,7 +6345,7 @@
       </c>
       <c r="I43" s="119" t="str">
         <f>_xll.qlBTP2(C43,,D43,E43,F43,G43,H43,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004712748#0001</v>
+        <v>IT0004712748#0003</v>
       </c>
       <c r="J43" s="127" t="b">
         <v>1</v>
@@ -6383,7 +6390,7 @@
       </c>
       <c r="I44" s="119" t="str">
         <f>_xll.qlBTP2(C44,,D44,E44,F44,G44,H44,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004917792#0001</v>
+        <v>IT0004917792#0003</v>
       </c>
       <c r="J44" s="127" t="b">
         <f t="shared" si="1"/>
@@ -6429,7 +6436,7 @@
       </c>
       <c r="I45" s="119" t="str">
         <f>_xll.qlBTP2(C45,,D45,E45,F45,G45,H45,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004019581#0001</v>
+        <v>IT0004019581#0003</v>
       </c>
       <c r="J45" s="127" t="b">
         <f t="shared" si="1"/>
@@ -6475,7 +6482,7 @@
       </c>
       <c r="I46" s="119" t="str">
         <f>_xll.qlBTP2(C46,,D46,E46,F46,G46,H46,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004761950#0001</v>
+        <v>IT0004761950#0003</v>
       </c>
       <c r="J46" s="127" t="b">
         <v>1</v>
@@ -6517,7 +6524,7 @@
       </c>
       <c r="I47" s="119" t="str">
         <f>_xll.qlBTP2(C47,,D47,E47,F47,G47,H47,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004960826#0001</v>
+        <v>IT0004960826#0003</v>
       </c>
       <c r="J47" s="127" t="b">
         <f t="shared" si="1"/>
@@ -6560,7 +6567,7 @@
       </c>
       <c r="I48" s="119" t="str">
         <f>_xll.qlBTP2(C48,,D48,E48,F48,G48,H48,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004987191#0001</v>
+        <v>IT0004987191#0003</v>
       </c>
       <c r="J48" s="127" t="b">
         <f t="shared" si="1"/>
@@ -6606,7 +6613,7 @@
       </c>
       <c r="I49" s="119" t="str">
         <f>_xll.qlBTP2(C49,,D49,E49,F49,G49,H49,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004164775#0001</v>
+        <v>IT0004164775#0003</v>
       </c>
       <c r="J49" s="127" t="b">
         <f t="shared" si="1"/>
@@ -6652,7 +6659,7 @@
       </c>
       <c r="I50" s="119" t="str">
         <f>_xll.qlBTP2(C50,,D50,E50,F50,G50,H50,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004793474#0001</v>
+        <v>IT0004793474#0003</v>
       </c>
       <c r="J50" s="127" t="b">
         <v>1</v>
@@ -6697,7 +6704,7 @@
       </c>
       <c r="I51" s="119" t="str">
         <f>_xll.qlBTP2(C51,,D51,E51,F51,G51,H51,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004820426#0001</v>
+        <v>IT0004820426#0003</v>
       </c>
       <c r="J51" s="127" t="b">
         <v>1</v>
@@ -6742,7 +6749,7 @@
       </c>
       <c r="I52" s="119" t="str">
         <f>_xll.qlBTP2(C52,,D52,E52,F52,G52,H52,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0003242747#0001</v>
+        <v>IT0003242747#0003</v>
       </c>
       <c r="J52" s="127" t="b">
         <f t="shared" si="1"/>
@@ -6788,7 +6795,7 @@
       </c>
       <c r="I53" s="119" t="str">
         <f>_xll.qlBTP2(C53,,D53,E53,F53,G53,H53,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004867070#0001</v>
+        <v>IT0004867070#0003</v>
       </c>
       <c r="J53" s="127" t="b">
         <v>1</v>
@@ -6833,7 +6840,7 @@
       </c>
       <c r="I54" s="119" t="str">
         <f>_xll.qlBTP2(C54,,D54,E54,F54,G54,H54,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004273493#0001</v>
+        <v>IT0004273493#0003</v>
       </c>
       <c r="J54" s="127" t="b">
         <f t="shared" si="1"/>
@@ -6879,7 +6886,7 @@
       </c>
       <c r="I55" s="119" t="str">
         <f>_xll.qlBTP2(C55,,D55,E55,F55,G55,H55,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004907843#0001</v>
+        <v>IT0004907843#0003</v>
       </c>
       <c r="J55" s="127" t="b">
         <v>1</v>
@@ -6924,7 +6931,7 @@
       </c>
       <c r="I56" s="119" t="str">
         <f>_xll.qlBTP2(C56,,D56,E56,F56,G56,H56,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004361041#0001</v>
+        <v>IT0004361041#0003</v>
       </c>
       <c r="J56" s="127" t="b">
         <f t="shared" si="1"/>
@@ -6967,7 +6974,7 @@
       </c>
       <c r="I57" s="119" t="str">
         <f>_xll.qlBTP2(C57,,D57,E57,F57,G57,H57,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004957574#0001</v>
+        <v>IT0004957574#0003</v>
       </c>
       <c r="J57" s="127" t="b">
         <v>1</v>
@@ -7012,7 +7019,7 @@
       </c>
       <c r="I58" s="119" t="str">
         <f>_xll.qlBTP2(C58,,D58,E58,F58,G58,H58,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0003493258#0001</v>
+        <v>IT0003493258#0003</v>
       </c>
       <c r="J58" s="127" t="b">
         <f t="shared" si="1"/>
@@ -7058,7 +7065,7 @@
       </c>
       <c r="I59" s="119" t="str">
         <f>_xll.qlBTP2(C59,,D59,E59,F59,G59,H59,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004423957#0001</v>
+        <v>IT0004423957#0003</v>
       </c>
       <c r="J59" s="127" t="b">
         <f t="shared" si="1"/>
@@ -7101,7 +7108,7 @@
       </c>
       <c r="I60" s="119" t="str">
         <f>_xll.qlBTP2(C60,,D60,E60,F60,G60,H60,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004992308#0001</v>
+        <v>IT0004992308#0003</v>
       </c>
       <c r="J60" s="127" t="b">
         <f t="shared" si="1"/>
@@ -7144,7 +7151,7 @@
       </c>
       <c r="I61" s="119" t="str">
         <f>_xll.qlBTP2(C61,,D61,E61,F61,G61,H61,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0005030504#0001</v>
+        <v>IT0005030504#0003</v>
       </c>
       <c r="J61" s="127" t="b">
         <v>0</v>
@@ -7189,7 +7196,7 @@
       </c>
       <c r="I62" s="119" t="str">
         <f>_xll.qlBTP2(C62,,D62,E62,F62,G62,H62,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004489610#0001</v>
+        <v>IT0004489610#0003</v>
       </c>
       <c r="J62" s="127" t="b">
         <f t="shared" si="1"/>
@@ -7235,7 +7242,7 @@
       </c>
       <c r="I63" s="119" t="str">
         <f>_xll.qlBTP2(C63,,D63,E63,F63,G63,H63,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0005069395#0002</v>
+        <v>IT0005069395#0003</v>
       </c>
       <c r="J63" s="127" t="b">
         <v>0</v>
@@ -7280,7 +7287,7 @@
       </c>
       <c r="I64" s="119" t="str">
         <f>_xll.qlBTP2(C64,,D64,E64,F64,G64,H64,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0003644769#0001</v>
+        <v>IT0003644769#0003</v>
       </c>
       <c r="J64" s="127" t="b">
         <f t="shared" si="1"/>
@@ -7326,7 +7333,7 @@
       </c>
       <c r="I65" s="119" t="str">
         <f>_xll.qlBTP2(C65,,D65,E65,F65,G65,H65,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004536949#0001</v>
+        <v>IT0004536949#0003</v>
       </c>
       <c r="J65" s="127" t="b">
         <f t="shared" si="1"/>
@@ -7372,7 +7379,7 @@
       </c>
       <c r="I66" s="119" t="str">
         <f>_xll.qlBTP2(C66,,D66,E66,F66,G66,H66,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004594930#0001</v>
+        <v>IT0004594930#0003</v>
       </c>
       <c r="J66" s="127" t="b">
         <v>1</v>
@@ -7417,7 +7424,7 @@
       </c>
       <c r="I67" s="119" t="str">
         <f>_xll.qlBTP2(C67,,D67,E67,F67,G67,H67,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004634132#0001</v>
+        <v>IT0004634132#0003</v>
       </c>
       <c r="J67" s="127" t="b">
         <f t="shared" si="1"/>
@@ -7461,7 +7468,7 @@
       </c>
       <c r="I68" s="119" t="str">
         <f>_xll.qlBTP2(C68,,D68,E68,F68,G68,H68,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004966401#0001</v>
+        <v>IT0004966401#0003</v>
       </c>
       <c r="J68" s="127" t="b">
         <v>1</v>
@@ -7507,7 +7514,7 @@
       </c>
       <c r="I69" s="119" t="str">
         <f>_xll.qlBTP2(C69,,D69,E69,F69,G69,H69,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004009673#0001</v>
+        <v>IT0004009673#0003</v>
       </c>
       <c r="J69" s="127" t="b">
         <f t="shared" si="1"/>
@@ -7554,7 +7561,7 @@
       </c>
       <c r="I70" s="119" t="str">
         <f>_xll.qlBTP2(C70,,D70,E70,F70,G70,H70,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004695075#0001</v>
+        <v>IT0004695075#0003</v>
       </c>
       <c r="J70" s="127" t="b">
         <f t="shared" si="1"/>
@@ -7598,7 +7605,7 @@
       </c>
       <c r="I71" s="119" t="str">
         <f>_xll.qlBTP2(C71,,D71,E71,F71,G71,H71,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0005028003#0001</v>
+        <v>IT0005028003#0003</v>
       </c>
       <c r="J71" s="127" t="b">
         <v>0</v>
@@ -7644,7 +7651,7 @@
       </c>
       <c r="I72" s="119" t="str">
         <f>_xll.qlBTP2(C72,,D72,E72,F72,G72,H72,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004759673#0001</v>
+        <v>IT0004759673#0003</v>
       </c>
       <c r="J72" s="127" t="b">
         <f t="shared" si="1"/>
@@ -7667,39 +7674,36 @@
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A73" s="19"/>
-      <c r="B73" s="126" t="str">
-        <f>_xll.ohRangeRetrieveError(I73)</f>
-        <v/>
-      </c>
+      <c r="B73" s="126"/>
       <c r="C73" s="40" t="s">
-        <v>430</v>
+        <v>456</v>
       </c>
       <c r="D73" s="85">
-        <v>44805</v>
+        <v>44666</v>
       </c>
       <c r="E73" s="86">
-        <v>5.5E-2</v>
+        <v>1.35E-2</v>
       </c>
       <c r="F73" s="87">
         <v>100</v>
       </c>
       <c r="G73" s="85">
-        <v>40969</v>
+        <v>42051</v>
       </c>
       <c r="H73" s="85">
-        <v>40969</v>
+        <v>42051</v>
       </c>
       <c r="I73" s="119" t="str">
         <f>_xll.qlBTP2(C73,,D73,E73,F73,G73,H73,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004801541#0001</v>
+        <v>IT0005086886#0000</v>
       </c>
       <c r="J73" s="127" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K73" s="121" t="str">
-        <f t="shared" si="0"/>
-        <v>Residual Missing</v>
+        <f t="shared" ref="K73" si="3">IF(AND(J73,ISNA(L73),ISNA(M73)),"Residual Missing","--")</f>
+        <v>--</v>
       </c>
       <c r="L73" s="48" t="e">
         <f>LEFT(VLOOKUP($D73,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
@@ -7719,10 +7723,10 @@
         <v/>
       </c>
       <c r="C74" s="40" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D74" s="85">
-        <v>44866</v>
+        <v>44805</v>
       </c>
       <c r="E74" s="86">
         <v>5.5E-2</v>
@@ -7731,14 +7735,14 @@
         <v>100</v>
       </c>
       <c r="G74" s="85">
-        <v>41030</v>
+        <v>40969</v>
       </c>
       <c r="H74" s="85">
-        <v>41155</v>
+        <v>40969</v>
       </c>
       <c r="I74" s="119" t="str">
         <f>_xll.qlBTP2(C74,,D74,E74,F74,G74,H74,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004848831#0001</v>
+        <v>IT0004801541#0003</v>
       </c>
       <c r="J74" s="127" t="b">
         <f t="shared" si="1"/>
@@ -7766,28 +7770,29 @@
         <v/>
       </c>
       <c r="C75" s="40" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="D75" s="85">
-        <v>45047</v>
+        <v>44866</v>
       </c>
       <c r="E75" s="86">
-        <v>4.4999999999999998E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="F75" s="87">
         <v>100</v>
       </c>
       <c r="G75" s="85">
-        <v>41334</v>
+        <v>41030</v>
       </c>
       <c r="H75" s="85">
-        <v>41334</v>
+        <v>41155</v>
       </c>
       <c r="I75" s="119" t="str">
         <f>_xll.qlBTP2(C75,,D75,E75,F75,G75,H75,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004898034#0001</v>
+        <v>IT0004848831#0003</v>
       </c>
       <c r="J75" s="127" t="b">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K75" s="121" t="str">
@@ -7812,42 +7817,41 @@
         <v/>
       </c>
       <c r="C76" s="40" t="s">
-        <v>50</v>
+        <v>438</v>
       </c>
       <c r="D76" s="85">
-        <v>45139</v>
+        <v>45047</v>
       </c>
       <c r="E76" s="86">
-        <v>4.7500000000000001E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="F76" s="87">
         <v>100</v>
       </c>
       <c r="G76" s="85">
-        <v>39479</v>
+        <v>41334</v>
       </c>
       <c r="H76" s="85">
-        <v>39554</v>
+        <v>41334</v>
       </c>
       <c r="I76" s="119" t="str">
         <f>_xll.qlBTP2(C76,,D76,E76,F76,G76,H76,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004356843#0001</v>
+        <v>IT0004898034#0003</v>
       </c>
       <c r="J76" s="127" t="b">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K76" s="121" t="str">
         <f t="shared" si="0"/>
-        <v>--</v>
+        <v>Residual Missing</v>
       </c>
       <c r="L76" s="48" t="e">
         <f>LEFT(VLOOKUP($D76,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
         <v>#N/A</v>
       </c>
-      <c r="M76" s="120" t="str">
+      <c r="M76" s="120" t="e">
         <f>LEFT(VLOOKUP($D76,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
-        <v>IT0004359029</v>
+        <v>#N/A</v>
       </c>
       <c r="N76" s="27"/>
       <c r="O76" s="18"/>
@@ -7859,81 +7863,85 @@
         <v/>
       </c>
       <c r="C77" s="40" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D77" s="85">
-        <v>45231</v>
+        <v>45139</v>
       </c>
       <c r="E77" s="86">
-        <v>0.09</v>
+        <v>4.7500000000000001E-2</v>
       </c>
       <c r="F77" s="87">
-        <v>99.909000000000006</v>
+        <v>100</v>
       </c>
       <c r="G77" s="85">
-        <v>34274</v>
+        <v>39479</v>
       </c>
       <c r="H77" s="85">
-        <v>34291</v>
+        <v>39554</v>
       </c>
       <c r="I77" s="119" t="str">
         <f>_xll.qlBTP2(C77,,D77,E77,F77,G77,H77,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0000366655#0001</v>
+        <v>IT0004356843#0003</v>
       </c>
       <c r="J77" s="127" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K77" s="121" t="str">
-        <f t="shared" ref="K77:K94" si="3">IF(AND(J77,ISNA(L77),ISNA(M77)),"Residual Missing","--")</f>
+        <f t="shared" si="0"/>
         <v>--</v>
       </c>
-      <c r="L77" s="48" t="str">
+      <c r="L77" s="48" t="e">
         <f>LEFT(VLOOKUP($D77,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
-        <v>IT0001246799</v>
-      </c>
-      <c r="M77" s="120" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M77" s="120" t="str">
         <f>LEFT(VLOOKUP($D77,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
-        <v>#N/A</v>
+        <v>IT0004359029</v>
       </c>
       <c r="N77" s="27"/>
       <c r="O77" s="18"/>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A78" s="19"/>
-      <c r="B78" s="126"/>
+      <c r="B78" s="126" t="str">
+        <f>_xll.ohRangeRetrieveError(I78)</f>
+        <v/>
+      </c>
       <c r="C78" s="40" t="s">
-        <v>441</v>
+        <v>46</v>
       </c>
       <c r="D78" s="85">
-        <v>45352</v>
+        <v>45231</v>
       </c>
       <c r="E78" s="86">
-        <v>4.4999999999999998E-2</v>
+        <v>0.09</v>
       </c>
       <c r="F78" s="87">
-        <v>100</v>
+        <v>99.909000000000006</v>
       </c>
       <c r="G78" s="85">
-        <v>41487</v>
+        <v>34274</v>
       </c>
       <c r="H78" s="85">
-        <v>41487</v>
+        <v>34291</v>
       </c>
       <c r="I78" s="119" t="str">
         <f>_xll.qlBTP2(C78,,D78,E78,F78,G78,H78,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004953417#0001</v>
+        <v>IT0000366655#0003</v>
       </c>
       <c r="J78" s="127" t="b">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K78" s="121" t="str">
-        <f>IF(AND(J78,ISNA(L78),ISNA(M78)),"Residual Missing","--")</f>
-        <v>Residual Missing</v>
-      </c>
-      <c r="L78" s="48" t="e">
+        <f t="shared" ref="K78:K97" si="4">IF(AND(J78,ISNA(L78),ISNA(M78)),"Residual Missing","--")</f>
+        <v>--</v>
+      </c>
+      <c r="L78" s="48" t="str">
         <f>LEFT(VLOOKUP($D78,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
-        <v>#N/A</v>
+        <v>IT0001246799</v>
       </c>
       <c r="M78" s="120" t="e">
         <f>LEFT(VLOOKUP($D78,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
@@ -7946,26 +7954,26 @@
       <c r="A79" s="19"/>
       <c r="B79" s="126"/>
       <c r="C79" s="40" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
       <c r="D79" s="85">
-        <v>45536</v>
+        <v>45352</v>
       </c>
       <c r="E79" s="86">
-        <v>3.7499999999999999E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="F79" s="87">
         <v>100</v>
       </c>
       <c r="G79" s="85">
-        <v>41699</v>
+        <v>41487</v>
       </c>
       <c r="H79" s="85">
-        <v>41701</v>
+        <v>41487</v>
       </c>
       <c r="I79" s="119" t="str">
         <f>_xll.qlBTP2(C79,,D79,E79,F79,G79,H79,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0005001547#0001</v>
+        <v>IT0004953417#0003</v>
       </c>
       <c r="J79" s="127" t="b">
         <v>1</v>
@@ -7989,26 +7997,26 @@
       <c r="A80" s="19"/>
       <c r="B80" s="126"/>
       <c r="C80" s="40" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="D80" s="85">
-        <v>45627</v>
+        <v>45536</v>
       </c>
       <c r="E80" s="86">
-        <v>2.5000000000000001E-2</v>
+        <v>3.7499999999999999E-2</v>
       </c>
       <c r="F80" s="87">
         <v>100</v>
       </c>
       <c r="G80" s="85">
-        <v>41883</v>
+        <v>41699</v>
       </c>
       <c r="H80" s="85">
-        <v>41883</v>
+        <v>41701</v>
       </c>
       <c r="I80" s="119" t="str">
         <f>_xll.qlBTP2(C80,,D80,E80,F80,G80,H80,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0005045270#0001</v>
+        <v>IT0005001547#0003</v>
       </c>
       <c r="J80" s="127" t="b">
         <v>1</v>
@@ -8030,37 +8038,34 @@
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A81" s="19"/>
-      <c r="B81" s="126" t="str">
-        <f>_xll.ohRangeRetrieveError(I81)</f>
-        <v/>
-      </c>
+      <c r="B81" s="126"/>
       <c r="C81" s="40" t="s">
-        <v>70</v>
+        <v>451</v>
       </c>
       <c r="D81" s="85">
-        <v>45717</v>
+        <v>45627</v>
       </c>
       <c r="E81" s="86">
-        <v>0.05</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="F81" s="87">
         <v>100</v>
       </c>
       <c r="G81" s="85">
-        <v>39873</v>
+        <v>41883</v>
       </c>
       <c r="H81" s="85">
-        <v>40009</v>
+        <v>41883</v>
       </c>
       <c r="I81" s="119" t="str">
         <f>_xll.qlBTP2(C81,,D81,E81,F81,G81,H81,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004513641#0001</v>
+        <v>IT0005045270#0003</v>
       </c>
       <c r="J81" s="127" t="b">
         <v>1</v>
       </c>
       <c r="K81" s="121" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(AND(J81,ISNA(L81),ISNA(M81)),"Residual Missing","--")</f>
         <v>Residual Missing</v>
       </c>
       <c r="L81" s="48" t="e">
@@ -8081,33 +8086,32 @@
         <v/>
       </c>
       <c r="C82" s="40" t="s">
-        <v>410</v>
+        <v>70</v>
       </c>
       <c r="D82" s="85">
-        <v>46082</v>
+        <v>45717</v>
       </c>
       <c r="E82" s="86">
-        <v>4.4999999999999998E-2</v>
+        <v>0.05</v>
       </c>
       <c r="F82" s="87">
         <v>100</v>
       </c>
       <c r="G82" s="85">
-        <v>40422</v>
+        <v>39873</v>
       </c>
       <c r="H82" s="85">
-        <v>40450</v>
+        <v>40009</v>
       </c>
       <c r="I82" s="119" t="str">
         <f>_xll.qlBTP2(C82,,D82,E82,F82,G82,H82,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004644735#0001</v>
+        <v>IT0004513641#0003</v>
       </c>
       <c r="J82" s="127" t="b">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K82" s="121" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Residual Missing</v>
       </c>
       <c r="L82" s="48" t="e">
@@ -8121,51 +8125,49 @@
       <c r="N82" s="27"/>
       <c r="O82" s="18"/>
     </row>
-    <row r="83" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A83" s="19"/>
-      <c r="B83" s="126" t="str">
-        <f>_xll.ohRangeRetrieveError(I83)</f>
-        <v/>
-      </c>
+      <c r="B83" s="126"/>
       <c r="C83" s="40" t="s">
-        <v>47</v>
+        <v>455</v>
       </c>
       <c r="D83" s="85">
-        <v>46327</v>
+        <v>45809</v>
       </c>
       <c r="E83" s="86">
-        <v>7.2499999999999995E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="F83" s="87">
-        <v>99.999000000000009</v>
+        <v>100</v>
       </c>
       <c r="G83" s="85">
-        <v>35370</v>
+        <v>42065</v>
       </c>
       <c r="H83" s="85">
-        <v>35464</v>
+        <v>42065</v>
       </c>
       <c r="I83" s="119" t="str">
         <f>_xll.qlBTP2(C83,,D83,E83,F83,G83,H83,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0001086567#0001</v>
+        <v>IT0005090318#0002</v>
       </c>
       <c r="J83" s="127" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K83" s="121" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="K83" si="5">IF(AND(J83,ISNA(L83),ISNA(M83)),"Residual Missing","--")</f>
         <v>--</v>
       </c>
-      <c r="L83" s="48" t="str">
+      <c r="L83" s="48" t="e">
         <f>LEFT(VLOOKUP($D83,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
-        <v>IT0001246807</v>
+        <v>#N/A</v>
       </c>
       <c r="M83" s="120" t="e">
         <f>LEFT(VLOOKUP($D83,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
         <v>#N/A</v>
       </c>
       <c r="N83" s="27"/>
+      <c r="O83" s="18"/>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A84" s="19"/>
@@ -8174,83 +8176,85 @@
         <v/>
       </c>
       <c r="C84" s="40" t="s">
-        <v>31</v>
+        <v>410</v>
       </c>
       <c r="D84" s="85">
-        <v>46692</v>
+        <v>46082</v>
       </c>
       <c r="E84" s="86">
-        <v>6.5000000000000002E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="F84" s="87">
         <v>100</v>
       </c>
       <c r="G84" s="85">
-        <v>35735</v>
+        <v>40422</v>
       </c>
       <c r="H84" s="85">
-        <v>35752</v>
+        <v>40450</v>
       </c>
       <c r="I84" s="119" t="str">
         <f>_xll.qlBTP2(C84,,D84,E84,F84,G84,H84,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0001174611#0001</v>
+        <v>IT0004644735#0003</v>
       </c>
       <c r="J84" s="127" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K84" s="121" t="str">
-        <f t="shared" si="3"/>
-        <v>--</v>
-      </c>
-      <c r="L84" s="48" t="str">
+        <f t="shared" si="4"/>
+        <v>Residual Missing</v>
+      </c>
+      <c r="L84" s="48" t="e">
         <f>LEFT(VLOOKUP($D84,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
-        <v>IT0001246815</v>
+        <v>#N/A</v>
       </c>
       <c r="M84" s="120" t="e">
         <f>LEFT(VLOOKUP($D84,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
         <v>#N/A</v>
       </c>
       <c r="N84" s="27"/>
-    </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O84" s="18"/>
+    </row>
+    <row r="85" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" s="19"/>
       <c r="B85" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(I85)</f>
         <v/>
       </c>
       <c r="C85" s="40" t="s">
-        <v>439</v>
+        <v>47</v>
       </c>
       <c r="D85" s="85">
-        <v>46997</v>
+        <v>46327</v>
       </c>
       <c r="E85" s="86">
-        <v>4.7500000000000001E-2</v>
+        <v>7.2499999999999995E-2</v>
       </c>
       <c r="F85" s="87">
-        <v>100</v>
+        <v>99.999000000000009</v>
       </c>
       <c r="G85" s="85">
-        <v>41296</v>
+        <v>35370</v>
       </c>
       <c r="H85" s="85">
-        <v>41296</v>
+        <v>35464</v>
       </c>
       <c r="I85" s="119" t="str">
         <f>_xll.qlBTP2(C85,,D85,E85,F85,G85,H85,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004889033#0001</v>
+        <v>IT0001086567#0003</v>
       </c>
       <c r="J85" s="127" t="b">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K85" s="121" t="str">
-        <f t="shared" si="3"/>
-        <v>Residual Missing</v>
-      </c>
-      <c r="L85" s="48" t="e">
+        <f t="shared" si="4"/>
+        <v>--</v>
+      </c>
+      <c r="L85" s="48" t="str">
         <f>LEFT(VLOOKUP($D85,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
-        <v>#N/A</v>
+        <v>IT0001246807</v>
       </c>
       <c r="M85" s="120" t="e">
         <f>LEFT(VLOOKUP($D85,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
@@ -8265,38 +8269,38 @@
         <v/>
       </c>
       <c r="C86" s="40" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D86" s="85">
-        <v>47423</v>
+        <v>46692</v>
       </c>
       <c r="E86" s="86">
-        <v>5.2499999999999998E-2</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="F86" s="87">
         <v>100</v>
       </c>
       <c r="G86" s="85">
-        <v>36100</v>
+        <v>35735</v>
       </c>
       <c r="H86" s="85">
-        <v>36117</v>
+        <v>35752</v>
       </c>
       <c r="I86" s="119" t="str">
         <f>_xll.qlBTP2(C86,,D86,E86,F86,G86,H86,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0001278511#0001</v>
+        <v>IT0001174611#0003</v>
       </c>
       <c r="J86" s="127" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K86" s="121" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>--</v>
       </c>
       <c r="L86" s="48" t="str">
         <f>LEFT(VLOOKUP($D86,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
-        <v>IT0001312773</v>
+        <v>IT0001246815</v>
       </c>
       <c r="M86" s="120" t="e">
         <f>LEFT(VLOOKUP($D86,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
@@ -8306,35 +8310,38 @@
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A87" s="19"/>
-      <c r="B87" s="126"/>
+      <c r="B87" s="126" t="str">
+        <f>_xll.ohRangeRetrieveError(I87)</f>
+        <v/>
+      </c>
       <c r="C87" s="40" t="s">
-        <v>450</v>
+        <v>439</v>
       </c>
       <c r="D87" s="85">
-        <v>47543</v>
+        <v>46997</v>
       </c>
       <c r="E87" s="86">
-        <v>3.5000000000000003E-2</v>
+        <v>4.7500000000000001E-2</v>
       </c>
       <c r="F87" s="87">
         <v>100</v>
       </c>
       <c r="G87" s="85">
-        <v>41699</v>
+        <v>41296</v>
       </c>
       <c r="H87" s="85">
-        <v>41699</v>
+        <v>41296</v>
       </c>
       <c r="I87" s="119" t="str">
         <f>_xll.qlBTP2(C87,,D87,E87,F87,G87,H87,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0005024234#0001</v>
+        <v>IT0004889033#0003</v>
       </c>
       <c r="J87" s="127" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K87" s="121" t="str">
-        <f>IF(AND(J87,ISNA(L87),ISNA(M87)),"Residual Missing","--")</f>
-        <v>--</v>
+        <f t="shared" si="4"/>
+        <v>Residual Missing</v>
       </c>
       <c r="L87" s="48" t="e">
         <f>LEFT(VLOOKUP($D87,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
@@ -8353,38 +8360,38 @@
         <v/>
       </c>
       <c r="C88" s="40" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D88" s="85">
-        <v>47969</v>
+        <v>47423</v>
       </c>
       <c r="E88" s="86">
-        <v>0.06</v>
+        <v>5.2499999999999998E-2</v>
       </c>
       <c r="F88" s="87">
         <v>100</v>
       </c>
       <c r="G88" s="85">
-        <v>36465</v>
+        <v>36100</v>
       </c>
       <c r="H88" s="85">
-        <v>36602</v>
+        <v>36117</v>
       </c>
       <c r="I88" s="119" t="str">
         <f>_xll.qlBTP2(C88,,D88,E88,F88,G88,H88,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0001444378#0001</v>
+        <v>IT0001278511#0003</v>
       </c>
       <c r="J88" s="127" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K88" s="121" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>--</v>
       </c>
       <c r="L88" s="48" t="str">
         <f>LEFT(VLOOKUP($D88,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
-        <v>IT0001464186</v>
+        <v>IT0001312773</v>
       </c>
       <c r="M88" s="120" t="e">
         <f>LEFT(VLOOKUP($D88,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
@@ -8394,47 +8401,43 @@
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A89" s="19"/>
-      <c r="B89" s="126" t="str">
-        <f>_xll.ohRangeRetrieveError(I89)</f>
-        <v/>
-      </c>
+      <c r="B89" s="126"/>
       <c r="C89" s="40" t="s">
-        <v>48</v>
+        <v>450</v>
       </c>
       <c r="D89" s="85">
-        <v>48611</v>
+        <v>47543</v>
       </c>
       <c r="E89" s="86">
-        <v>5.7500000000000002E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="F89" s="87">
         <v>100</v>
       </c>
       <c r="G89" s="85">
-        <v>37288</v>
+        <v>41699</v>
       </c>
       <c r="H89" s="85">
-        <v>37333</v>
+        <v>41699</v>
       </c>
       <c r="I89" s="119" t="str">
         <f>_xll.qlBTP2(C89,,D89,E89,F89,G89,H89,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0003256820#0001</v>
+        <v>IT0005024234#0003</v>
       </c>
       <c r="J89" s="127" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K89" s="121" t="str">
-        <f t="shared" si="3"/>
+        <f>IF(AND(J89,ISNA(L89),ISNA(M89)),"Residual Missing","--")</f>
         <v>--</v>
       </c>
       <c r="L89" s="48" t="e">
         <f>LEFT(VLOOKUP($D89,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
         <v>#N/A</v>
       </c>
-      <c r="M89" s="120" t="str">
+      <c r="M89" s="120" t="e">
         <f>LEFT(VLOOKUP($D89,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
-        <v>IT0003268460</v>
+        <v>#N/A</v>
       </c>
       <c r="N89" s="27"/>
     </row>
@@ -8445,42 +8448,42 @@
         <v/>
       </c>
       <c r="C90" s="40" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="D90" s="85">
-        <v>49157</v>
+        <v>47969</v>
       </c>
       <c r="E90" s="86">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="F90" s="87">
         <v>100</v>
       </c>
       <c r="G90" s="85">
-        <v>37834</v>
+        <v>36465</v>
       </c>
       <c r="H90" s="85">
-        <v>37888</v>
+        <v>36602</v>
       </c>
       <c r="I90" s="119" t="str">
         <f>_xll.qlBTP2(C90,,D90,E90,F90,G90,H90,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0003535157#0001</v>
+        <v>IT0001444378#0003</v>
       </c>
       <c r="J90" s="127" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K90" s="121" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>--</v>
       </c>
-      <c r="L90" s="48" t="e">
+      <c r="L90" s="48" t="str">
         <f>LEFT(VLOOKUP($D90,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M90" s="120" t="str">
+        <v>IT0001464186</v>
+      </c>
+      <c r="M90" s="120" t="e">
         <f>LEFT(VLOOKUP($D90,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
-        <v>IT0003540371</v>
+        <v>#N/A</v>
       </c>
       <c r="N90" s="27"/>
     </row>
@@ -8491,33 +8494,33 @@
         <v/>
       </c>
       <c r="C91" s="40" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="D91" s="85">
-        <v>50072</v>
+        <v>48611</v>
       </c>
       <c r="E91" s="86">
-        <v>0.04</v>
+        <v>5.7500000000000002E-2</v>
       </c>
       <c r="F91" s="87">
         <v>100</v>
       </c>
       <c r="G91" s="85">
-        <v>38565</v>
+        <v>37288</v>
       </c>
       <c r="H91" s="85">
-        <v>38644</v>
+        <v>37333</v>
       </c>
       <c r="I91" s="119" t="str">
         <f>_xll.qlBTP2(C91,,D91,E91,F91,G91,H91,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0003934657#0001</v>
+        <v>IT0003256820#0003</v>
       </c>
       <c r="J91" s="127" t="b">
-        <f>NOT(ISNA(VLOOKUP(LEFT($I91,12),LatestStrippable,1,FALSE)))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K91" s="121" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>--</v>
       </c>
       <c r="L91" s="48" t="e">
@@ -8526,7 +8529,7 @@
       </c>
       <c r="M91" s="120" t="str">
         <f>LEFT(VLOOKUP($D91,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
-        <v>IT0004002801</v>
+        <v>IT0003268460</v>
       </c>
       <c r="N91" s="27"/>
     </row>
@@ -8537,10 +8540,10 @@
         <v/>
       </c>
       <c r="C92" s="40" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="D92" s="85">
-        <v>50983</v>
+        <v>49157</v>
       </c>
       <c r="E92" s="86">
         <v>0.05</v>
@@ -8549,21 +8552,21 @@
         <v>100</v>
       </c>
       <c r="G92" s="85">
-        <v>39295</v>
+        <v>37834</v>
       </c>
       <c r="H92" s="85">
-        <v>39378</v>
+        <v>37888</v>
       </c>
       <c r="I92" s="119" t="str">
         <f>_xll.qlBTP2(C92,,D92,E92,F92,G92,H92,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004286966#0001</v>
+        <v>IT0003535157#0003</v>
       </c>
       <c r="J92" s="127" t="b">
-        <f>NOT(ISNA(VLOOKUP(LEFT($I92,12),LatestStrippable,1,FALSE)))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K92" s="121" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>--</v>
       </c>
       <c r="L92" s="48" t="e">
@@ -8572,155 +8575,290 @@
       </c>
       <c r="M92" s="120" t="str">
         <f>LEFT(VLOOKUP($D92,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
-        <v>IT0004288574</v>
+        <v>IT0003540371</v>
       </c>
       <c r="N92" s="27"/>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A93" s="19"/>
-      <c r="B93" s="126"/>
+      <c r="B93" s="126" t="str">
+        <f>_xll.ohRangeRetrieveError(I93)</f>
+        <v/>
+      </c>
       <c r="C93" s="40" t="s">
-        <v>71</v>
+        <v>15</v>
       </c>
       <c r="D93" s="85">
-        <v>51380</v>
+        <v>50072</v>
       </c>
       <c r="E93" s="86">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="F93" s="87">
         <v>100</v>
       </c>
       <c r="G93" s="85">
-        <v>40057</v>
+        <v>38565</v>
       </c>
       <c r="H93" s="85">
-        <v>40072</v>
+        <v>38644</v>
       </c>
       <c r="I93" s="119" t="str">
         <f>_xll.qlBTP2(C93,,D93,E93,F93,G93,H93,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004532559#0001</v>
+        <v>IT0003934657#0003</v>
       </c>
       <c r="J93" s="127" t="b">
         <f>NOT(ISNA(VLOOKUP(LEFT($I93,12),LatestStrippable,1,FALSE)))</f>
         <v>1</v>
       </c>
       <c r="K93" s="121" t="str">
-        <f>IF(AND(J93,ISNA(L93),ISNA(M93)),"Residual Missing","--")</f>
-        <v>Residual Missing</v>
+        <f t="shared" si="4"/>
+        <v>--</v>
       </c>
       <c r="L93" s="48" t="e">
         <f>LEFT(VLOOKUP($D93,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
         <v>#N/A</v>
       </c>
-      <c r="M93" s="120" t="e">
+      <c r="M93" s="120" t="str">
         <f>LEFT(VLOOKUP($D93,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
-        <v>#N/A</v>
+        <v>IT0004002801</v>
       </c>
       <c r="N93" s="27"/>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A94" s="19"/>
-      <c r="B94" s="128" t="str">
+      <c r="B94" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(I94)</f>
         <v/>
       </c>
-      <c r="C94" s="129" t="s">
-        <v>440</v>
-      </c>
-      <c r="D94" s="130">
-        <v>52841</v>
-      </c>
-      <c r="E94" s="131">
-        <v>4.7500000000000001E-2</v>
-      </c>
-      <c r="F94" s="132">
-        <v>100</v>
-      </c>
-      <c r="G94" s="130">
-        <v>41334</v>
-      </c>
-      <c r="H94" s="130">
-        <v>41416</v>
-      </c>
-      <c r="I94" s="133" t="str">
+      <c r="C94" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="D94" s="85">
+        <v>50983</v>
+      </c>
+      <c r="E94" s="86">
+        <v>0.05</v>
+      </c>
+      <c r="F94" s="87">
+        <v>100</v>
+      </c>
+      <c r="G94" s="85">
+        <v>39295</v>
+      </c>
+      <c r="H94" s="85">
+        <v>39378</v>
+      </c>
+      <c r="I94" s="119" t="str">
         <f>_xll.qlBTP2(C94,,D94,E94,F94,G94,H94,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004923998#0001</v>
-      </c>
-      <c r="J94" s="134" t="b">
+        <v>IT0004286966#0003</v>
+      </c>
+      <c r="J94" s="127" t="b">
+        <f>NOT(ISNA(VLOOKUP(LEFT($I94,12),LatestStrippable,1,FALSE)))</f>
         <v>1</v>
       </c>
       <c r="K94" s="121" t="str">
-        <f t="shared" si="3"/>
-        <v>Residual Missing</v>
-      </c>
-      <c r="L94" s="136" t="e">
+        <f t="shared" si="4"/>
+        <v>--</v>
+      </c>
+      <c r="L94" s="48" t="e">
         <f>LEFT(VLOOKUP($D94,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
         <v>#N/A</v>
       </c>
-      <c r="M94" s="120" t="e">
+      <c r="M94" s="120" t="str">
         <f>LEFT(VLOOKUP($D94,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
-        <v>#N/A</v>
+        <v>IT0004288574</v>
       </c>
       <c r="N94" s="27"/>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A95" s="19"/>
-      <c r="B95" s="49"/>
-      <c r="C95" s="49"/>
-      <c r="D95" s="49"/>
-      <c r="E95" s="49"/>
-      <c r="F95" s="49"/>
-      <c r="G95" s="49"/>
-      <c r="H95" s="49"/>
-      <c r="I95" s="49"/>
-      <c r="J95" s="49"/>
-      <c r="K95" s="22"/>
-      <c r="L95" s="49"/>
-      <c r="M95" s="49"/>
+      <c r="B95" s="126"/>
+      <c r="C95" s="40" t="s">
+        <v>71</v>
+      </c>
+      <c r="D95" s="85">
+        <v>51380</v>
+      </c>
+      <c r="E95" s="86">
+        <v>0.05</v>
+      </c>
+      <c r="F95" s="87">
+        <v>100</v>
+      </c>
+      <c r="G95" s="85">
+        <v>40057</v>
+      </c>
+      <c r="H95" s="85">
+        <v>40072</v>
+      </c>
+      <c r="I95" s="119" t="str">
+        <f>_xll.qlBTP2(C95,,D95,E95,F95,G95,H95,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>IT0004532559#0003</v>
+      </c>
+      <c r="J95" s="127" t="b">
+        <f>NOT(ISNA(VLOOKUP(LEFT($I95,12),LatestStrippable,1,FALSE)))</f>
+        <v>1</v>
+      </c>
+      <c r="K95" s="121" t="str">
+        <f>IF(AND(J95,ISNA(L95),ISNA(M95)),"Residual Missing","--")</f>
+        <v>Residual Missing</v>
+      </c>
+      <c r="L95" s="48" t="e">
+        <f>LEFT(VLOOKUP($D95,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M95" s="120" t="e">
+        <f>LEFT(VLOOKUP($D95,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
+        <v>#N/A</v>
+      </c>
       <c r="N95" s="27"/>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A96" s="19"/>
-      <c r="B96" s="22"/>
-      <c r="C96" s="22"/>
-      <c r="D96" s="22"/>
-      <c r="E96" s="22"/>
-      <c r="F96" s="22"/>
-      <c r="G96" s="22"/>
-      <c r="H96" s="22"/>
-      <c r="I96" s="22" t="str">
-        <f>_xll.ohGroup(J96,_xll.ohFilter(I8:I94,J8:J94),Permanent,,ObjectOverwrite)</f>
-        <v>StrippableBTPs#0005</v>
-      </c>
-      <c r="J96" s="22" t="s">
+      <c r="B96" s="126" t="str">
+        <f>_xll.ohRangeRetrieveError(I96)</f>
+        <v/>
+      </c>
+      <c r="C96" s="40" t="s">
+        <v>440</v>
+      </c>
+      <c r="D96" s="85">
+        <v>52841</v>
+      </c>
+      <c r="E96" s="86">
+        <v>4.7500000000000001E-2</v>
+      </c>
+      <c r="F96" s="87">
+        <v>100</v>
+      </c>
+      <c r="G96" s="85">
+        <v>41334</v>
+      </c>
+      <c r="H96" s="85">
+        <v>41416</v>
+      </c>
+      <c r="I96" s="119" t="str">
+        <f>_xll.qlBTP2(C96,,D96,E96,F96,G96,H96,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>IT0004923998#0003</v>
+      </c>
+      <c r="J96" s="127" t="b">
+        <v>1</v>
+      </c>
+      <c r="K96" s="121" t="str">
+        <f t="shared" si="4"/>
+        <v>Residual Missing</v>
+      </c>
+      <c r="L96" s="48" t="e">
+        <f>LEFT(VLOOKUP($D96,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M96" s="120" t="e">
+        <f>LEFT(VLOOKUP($D96,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N96" s="27"/>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A97" s="19"/>
+      <c r="B97" s="128"/>
+      <c r="C97" s="129" t="s">
+        <v>454</v>
+      </c>
+      <c r="D97" s="130">
+        <v>53571</v>
+      </c>
+      <c r="E97" s="131">
+        <v>3.2500000000000001E-2</v>
+      </c>
+      <c r="F97" s="132">
+        <v>100</v>
+      </c>
+      <c r="G97" s="130">
+        <v>41883</v>
+      </c>
+      <c r="H97" s="130">
+        <v>42026</v>
+      </c>
+      <c r="I97" s="119" t="str">
+        <f>_xll.qlBTP2(C97,,D97,E97,F97,G97,H97,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>IT0005083057#0007</v>
+      </c>
+      <c r="J97" s="133" t="b">
+        <f>NOT(ISNA(VLOOKUP(LEFT($I97,12),LatestStrippable,1,FALSE)))</f>
+        <v>0</v>
+      </c>
+      <c r="K97" s="121" t="str">
+        <f t="shared" si="4"/>
+        <v>--</v>
+      </c>
+      <c r="L97" s="48" t="e">
+        <f>LEFT(VLOOKUP($D97,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M97" s="120" t="e">
+        <f>LEFT(VLOOKUP($D97,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N97" s="27"/>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A98" s="19"/>
+      <c r="B98" s="49"/>
+      <c r="C98" s="49"/>
+      <c r="D98" s="49"/>
+      <c r="E98" s="49"/>
+      <c r="F98" s="49"/>
+      <c r="G98" s="49"/>
+      <c r="H98" s="49"/>
+      <c r="I98" s="49"/>
+      <c r="J98" s="49"/>
+      <c r="K98" s="22"/>
+      <c r="L98" s="49"/>
+      <c r="M98" s="49"/>
+      <c r="N98" s="27"/>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A99" s="19"/>
+      <c r="B99" s="22"/>
+      <c r="C99" s="22"/>
+      <c r="D99" s="22"/>
+      <c r="E99" s="22"/>
+      <c r="F99" s="22"/>
+      <c r="G99" s="22"/>
+      <c r="H99" s="22"/>
+      <c r="I99" s="22" t="str">
+        <f>_xll.ohGroup(J99,_xll.ohFilter(I8:I96,J8:J96),Permanent,,ObjectOverwrite)</f>
+        <v>StrippableBTPs#0008</v>
+      </c>
+      <c r="J99" s="22" t="s">
         <v>357</v>
       </c>
-      <c r="K96" s="22"/>
-      <c r="L96" s="22"/>
-      <c r="M96" s="22"/>
-      <c r="N96" s="27"/>
-    </row>
-    <row r="97" spans="1:14" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="44"/>
-      <c r="B97" s="45"/>
-      <c r="C97" s="45"/>
-      <c r="D97" s="45"/>
-      <c r="E97" s="45"/>
-      <c r="F97" s="45"/>
-      <c r="G97" s="45"/>
-      <c r="H97" s="45"/>
-      <c r="I97" s="45" t="str">
-        <f>_xll.ohGroup(J97,I8:I94,Permanent,,ObjectOverwrite)</f>
-        <v>BTPs#0003</v>
-      </c>
-      <c r="J97" s="45" t="s">
+      <c r="K99" s="22"/>
+      <c r="L99" s="22"/>
+      <c r="M99" s="22"/>
+      <c r="N99" s="27"/>
+    </row>
+    <row r="100" spans="1:14" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="44"/>
+      <c r="B100" s="45"/>
+      <c r="C100" s="45"/>
+      <c r="D100" s="45"/>
+      <c r="E100" s="45"/>
+      <c r="F100" s="45"/>
+      <c r="G100" s="45"/>
+      <c r="H100" s="45"/>
+      <c r="I100" s="45" t="str">
+        <f>_xll.ohGroup(J100,I8:I96,Permanent,,ObjectOverwrite)</f>
+        <v>BTPs#0006</v>
+      </c>
+      <c r="J100" s="45" t="s">
         <v>356</v>
       </c>
-      <c r="K97" s="45"/>
-      <c r="L97" s="45"/>
-      <c r="M97" s="45"/>
-      <c r="N97" s="46"/>
+      <c r="K100" s="45"/>
+      <c r="L100" s="45"/>
+      <c r="M100" s="45"/>
+      <c r="N100" s="46"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -8771,7 +8909,7 @@
         <v>452</v>
       </c>
       <c r="B2" s="101" t="e">
-        <f>VLOOKUP(A2,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A2,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8780,7 +8918,7 @@
         <v>452</v>
       </c>
       <c r="B3" s="101" t="e">
-        <f>VLOOKUP(A3,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A3,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8789,7 +8927,7 @@
         <v>452</v>
       </c>
       <c r="B4" s="101" t="e">
-        <f>VLOOKUP(A4,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A4,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8798,7 +8936,7 @@
         <v>452</v>
       </c>
       <c r="B5" s="101" t="e">
-        <f>VLOOKUP(A5,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A5,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8807,7 +8945,7 @@
         <v>452</v>
       </c>
       <c r="B6" s="101" t="e">
-        <f>VLOOKUP(A6,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A6,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8816,7 +8954,7 @@
         <v>452</v>
       </c>
       <c r="B7" s="101" t="e">
-        <f>VLOOKUP(A7,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A7,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8825,7 +8963,7 @@
         <v>452</v>
       </c>
       <c r="B8" s="101" t="e">
-        <f>VLOOKUP(A8,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A8,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8834,7 +8972,7 @@
         <v>452</v>
       </c>
       <c r="B9" s="101" t="e">
-        <f>VLOOKUP(A9,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A9,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8843,7 +8981,7 @@
         <v>452</v>
       </c>
       <c r="B10" s="101" t="e">
-        <f>VLOOKUP(A10,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A10,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8852,7 +8990,7 @@
         <v>452</v>
       </c>
       <c r="B11" s="101" t="e">
-        <f>VLOOKUP(A11,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A11,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8861,7 +8999,7 @@
         <v>452</v>
       </c>
       <c r="B12" s="101" t="e">
-        <f>VLOOKUP(A12,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A12,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8870,7 +9008,7 @@
         <v>452</v>
       </c>
       <c r="B13" s="101" t="e">
-        <f>VLOOKUP(A13,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A13,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8879,7 +9017,7 @@
         <v>452</v>
       </c>
       <c r="B14" s="101" t="e">
-        <f>VLOOKUP(A14,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A14,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8888,7 +9026,7 @@
         <v>452</v>
       </c>
       <c r="B15" s="101" t="e">
-        <f>VLOOKUP(A15,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A15,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8897,7 +9035,7 @@
         <v>452</v>
       </c>
       <c r="B16" s="101" t="e">
-        <f>VLOOKUP(A16,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A16,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8906,7 +9044,7 @@
         <v>452</v>
       </c>
       <c r="B17" s="101" t="e">
-        <f>VLOOKUP(A17,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A17,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8915,7 +9053,7 @@
         <v>452</v>
       </c>
       <c r="B18" s="101" t="e">
-        <f>VLOOKUP(A18,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A18,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8924,7 +9062,7 @@
         <v>452</v>
       </c>
       <c r="B19" s="101" t="e">
-        <f>VLOOKUP(A19,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A19,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8933,7 +9071,7 @@
         <v>452</v>
       </c>
       <c r="B20" s="101" t="e">
-        <f>VLOOKUP(A20,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A20,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8942,7 +9080,7 @@
         <v>452</v>
       </c>
       <c r="B21" s="101" t="e">
-        <f>VLOOKUP(A21,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A21,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8951,7 +9089,7 @@
         <v>452</v>
       </c>
       <c r="B22" s="101" t="e">
-        <f>VLOOKUP(A22,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A22,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8960,7 +9098,7 @@
         <v>452</v>
       </c>
       <c r="B23" s="101" t="e">
-        <f>VLOOKUP(A23,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A23,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8969,7 +9107,7 @@
         <v>452</v>
       </c>
       <c r="B24" s="101" t="e">
-        <f>VLOOKUP(A24,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A24,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8978,7 +9116,7 @@
         <v>452</v>
       </c>
       <c r="B25" s="101" t="e">
-        <f>VLOOKUP(A25,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A25,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8987,7 +9125,7 @@
         <v>452</v>
       </c>
       <c r="B26" s="101" t="e">
-        <f>VLOOKUP(A26,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A26,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8996,7 +9134,7 @@
         <v>452</v>
       </c>
       <c r="B27" s="101" t="e">
-        <f>VLOOKUP(A27,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A27,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -9005,7 +9143,7 @@
         <v>452</v>
       </c>
       <c r="B28" s="101" t="e">
-        <f>VLOOKUP(A28,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A28,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -9014,7 +9152,7 @@
         <v>452</v>
       </c>
       <c r="B29" s="101" t="e">
-        <f>VLOOKUP(A29,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A29,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -9023,7 +9161,7 @@
         <v>452</v>
       </c>
       <c r="B30" s="101" t="e">
-        <f>VLOOKUP(A30,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A30,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -9032,7 +9170,7 @@
         <v>452</v>
       </c>
       <c r="B31" s="101" t="e">
-        <f>VLOOKUP(A31,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A31,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -9041,7 +9179,7 @@
         <v>452</v>
       </c>
       <c r="B32" s="101" t="e">
-        <f>VLOOKUP(A32,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A32,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -9050,7 +9188,7 @@
         <v>452</v>
       </c>
       <c r="B33" s="101" t="e">
-        <f>VLOOKUP(A33,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A33,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -9059,7 +9197,7 @@
         <v>452</v>
       </c>
       <c r="B34" s="101" t="e">
-        <f>VLOOKUP(A34,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A34,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -9068,7 +9206,7 @@
         <v>452</v>
       </c>
       <c r="B35" s="101" t="e">
-        <f>VLOOKUP(A35,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A35,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D35" s="102" t="str">
@@ -9126,7 +9264,7 @@
         <v>452</v>
       </c>
       <c r="B36" s="101" t="e">
-        <f>VLOOKUP(A36,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A36,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D36" s="103">
@@ -9196,7 +9334,7 @@
         <v>452</v>
       </c>
       <c r="B37" s="101" t="e">
-        <f>VLOOKUP(A37,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A37,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D37" s="103">
@@ -9266,7 +9404,7 @@
         <v>452</v>
       </c>
       <c r="B38" s="101" t="e">
-        <f>VLOOKUP(A38,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A38,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D38" s="103">
@@ -9336,7 +9474,7 @@
         <v>452</v>
       </c>
       <c r="B39" s="101" t="e">
-        <f>VLOOKUP(A39,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A39,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D39" s="103">
@@ -9406,7 +9544,7 @@
         <v>452</v>
       </c>
       <c r="B40" s="101" t="e">
-        <f>VLOOKUP(A40,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A40,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D40" s="103">
@@ -9476,7 +9614,7 @@
         <v>452</v>
       </c>
       <c r="B41" s="101" t="e">
-        <f>VLOOKUP(A41,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A41,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D41" s="103">
@@ -9546,7 +9684,7 @@
         <v>452</v>
       </c>
       <c r="B42" s="101" t="e">
-        <f>VLOOKUP(A42,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A42,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D42" s="103">
@@ -9616,7 +9754,7 @@
         <v>452</v>
       </c>
       <c r="B43" s="101" t="e">
-        <f>VLOOKUP(A43,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A43,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D43" s="103">
@@ -9686,7 +9824,7 @@
         <v>452</v>
       </c>
       <c r="B44" s="101" t="e">
-        <f>VLOOKUP(A44,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A44,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D44" s="103">
@@ -9756,7 +9894,7 @@
         <v>452</v>
       </c>
       <c r="B45" s="101" t="e">
-        <f>VLOOKUP(A45,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A45,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D45" s="103">
@@ -9826,7 +9964,7 @@
         <v>452</v>
       </c>
       <c r="B46" s="101" t="e">
-        <f>VLOOKUP(A46,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A46,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D46" s="103">
@@ -9896,7 +10034,7 @@
         <v>452</v>
       </c>
       <c r="B47" s="101" t="e">
-        <f>VLOOKUP(A47,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A47,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D47" s="103">
@@ -9966,7 +10104,7 @@
         <v>452</v>
       </c>
       <c r="B48" s="101" t="e">
-        <f>VLOOKUP(A48,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A48,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D48" s="103">
@@ -10036,7 +10174,7 @@
         <v>452</v>
       </c>
       <c r="B49" s="101" t="e">
-        <f>VLOOKUP(A49,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A49,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D49" s="103">
@@ -10106,7 +10244,7 @@
         <v>452</v>
       </c>
       <c r="B50" s="101" t="e">
-        <f>VLOOKUP(A50,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A50,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D50" s="103">
@@ -10176,7 +10314,7 @@
         <v>452</v>
       </c>
       <c r="B51" s="101" t="e">
-        <f>VLOOKUP(A51,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A51,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D51" s="103">
@@ -10246,7 +10384,7 @@
         <v>452</v>
       </c>
       <c r="B52" s="101" t="e">
-        <f>VLOOKUP(A52,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A52,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D52" s="103">
@@ -10316,7 +10454,7 @@
         <v>452</v>
       </c>
       <c r="B53" s="101" t="e">
-        <f>VLOOKUP(A53,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A53,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D53" s="103" t="e">
@@ -10367,7 +10505,7 @@
         <v>452</v>
       </c>
       <c r="B54" s="101" t="e">
-        <f>VLOOKUP(A54,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A54,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D54" s="103" t="e">
@@ -10418,7 +10556,7 @@
         <v>452</v>
       </c>
       <c r="B55" s="101" t="e">
-        <f>VLOOKUP(A55,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A55,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D55" s="103" t="e">
@@ -10469,7 +10607,7 @@
         <v>452</v>
       </c>
       <c r="B56" s="101" t="e">
-        <f>VLOOKUP(A56,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A56,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D56" s="103" t="e">
@@ -10520,7 +10658,7 @@
         <v>452</v>
       </c>
       <c r="B57" s="101" t="e">
-        <f>VLOOKUP(A57,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A57,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D57" s="103" t="e">
@@ -10571,7 +10709,7 @@
         <v>452</v>
       </c>
       <c r="B58" s="101" t="e">
-        <f>VLOOKUP(A58,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A58,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D58" s="103" t="e">
@@ -10622,7 +10760,7 @@
         <v>452</v>
       </c>
       <c r="B59" s="101" t="e">
-        <f>VLOOKUP(A59,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A59,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D59" s="103" t="e">
@@ -10673,7 +10811,7 @@
         <v>452</v>
       </c>
       <c r="B60" s="101" t="e">
-        <f>VLOOKUP(A60,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A60,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D60" s="103" t="e">
@@ -10724,7 +10862,7 @@
         <v>452</v>
       </c>
       <c r="B61" s="101" t="e">
-        <f>VLOOKUP(A61,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A61,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D61" s="103" t="e">
@@ -10775,7 +10913,7 @@
         <v>452</v>
       </c>
       <c r="B62" s="101" t="e">
-        <f>VLOOKUP(A62,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A62,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D62" s="103" t="e">
@@ -10826,7 +10964,7 @@
         <v>452</v>
       </c>
       <c r="B63" s="101" t="e">
-        <f>VLOOKUP(A63,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A63,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D63" s="103" t="e">
@@ -10877,7 +11015,7 @@
         <v>452</v>
       </c>
       <c r="B64" s="101" t="e">
-        <f>VLOOKUP(A64,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A64,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D64" s="103" t="e">
@@ -10928,7 +11066,7 @@
         <v>452</v>
       </c>
       <c r="B65" s="101" t="e">
-        <f>VLOOKUP(A65,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A65,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D65" s="103" t="e">
@@ -10979,7 +11117,7 @@
         <v>452</v>
       </c>
       <c r="B66" s="101" t="e">
-        <f>VLOOKUP(A66,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A66,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D66" s="103" t="e">
@@ -11030,7 +11168,7 @@
         <v>452</v>
       </c>
       <c r="B67" s="101" t="e">
-        <f>VLOOKUP(A67,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A67,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D67" s="103" t="e">
@@ -11081,7 +11219,7 @@
         <v>452</v>
       </c>
       <c r="B68" s="101" t="e">
-        <f>VLOOKUP(A68,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A68,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D68" s="103" t="e">
@@ -11132,7 +11270,7 @@
         <v>452</v>
       </c>
       <c r="B69" s="101" t="e">
-        <f>VLOOKUP(A69,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A69,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D69" s="103" t="e">
@@ -11183,7 +11321,7 @@
         <v>452</v>
       </c>
       <c r="B70" s="101" t="e">
-        <f>VLOOKUP(A70,BTP!$C$8:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A70,BTP!$C$8:$C$96,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D70" s="103" t="e">
@@ -13165,7 +13303,7 @@
         <v>IT0003106595</v>
       </c>
       <c r="P8" s="48" t="str">
-        <f>_xll.qlBondMaturityLookup("StrippableBTPs",$H8,BTP!$I$96)</f>
+        <f>_xll.qlBondMaturityLookup("StrippableBTPs",$H8,BTP!$I$99)</f>
         <v>IT0003080402</v>
       </c>
       <c r="Q8" s="23"/>
@@ -13216,7 +13354,7 @@
         <v>IT0003204945</v>
       </c>
       <c r="P9" s="48" t="str">
-        <f>_xll.qlBondMaturityLookup("StrippableBTPs",$H9,BTP!$I$96)</f>
+        <f>_xll.qlBondMaturityLookup("StrippableBTPs",$H9,BTP!$I$99)</f>
         <v>IT0003190912</v>
       </c>
       <c r="Q9" s="23"/>
@@ -13267,7 +13405,7 @@
         <v>IT0003246391</v>
       </c>
       <c r="P10" s="48" t="str">
-        <f>_xll.qlBondMaturityLookup("StrippableBTPs",$H10,BTP!$I$96)</f>
+        <f>_xll.qlBondMaturityLookup("StrippableBTPs",$H10,BTP!$I$99)</f>
         <v>IT0003357982</v>
       </c>
       <c r="Q10" s="23"/>
@@ -13318,7 +13456,7 @@
         <v>IT0003246383</v>
       </c>
       <c r="P11" s="48" t="str">
-        <f>_xll.qlBondMaturityLookup("StrippableBTPs",$H11,BTP!$I$96)</f>
+        <f>_xll.qlBondMaturityLookup("StrippableBTPs",$H11,BTP!$I$99)</f>
         <v>IT0003472336</v>
       </c>
       <c r="Q11" s="23"/>
@@ -13369,7 +13507,7 @@
         <v>IT0003246359</v>
       </c>
       <c r="P12" s="48" t="str">
-        <f>_xll.qlBondMaturityLookup("StrippableBTPs",$H12,BTP!$I$96)</f>
+        <f>_xll.qlBondMaturityLookup("StrippableBTPs",$H12,BTP!$I$99)</f>
         <v>IT0003618383</v>
       </c>
       <c r="Q12" s="23"/>
@@ -13420,7 +13558,7 @@
         <v>IT0003246342</v>
       </c>
       <c r="P13" s="48" t="str">
-        <f>_xll.qlBondMaturityLookup("StrippableBTPs",$H13,BTP!$I$96)</f>
+        <f>_xll.qlBondMaturityLookup("StrippableBTPs",$H13,BTP!$I$99)</f>
         <v>IT0003719918</v>
       </c>
       <c r="Q13" s="23"/>
@@ -13471,7 +13609,7 @@
         <v>IT0003246326</v>
       </c>
       <c r="P14" s="48" t="str">
-        <f>_xll.qlBondMaturityLookup("StrippableBTPs",$H14,BTP!$I$96)</f>
+        <f>_xll.qlBondMaturityLookup("StrippableBTPs",$H14,BTP!$I$99)</f>
         <v>IT0003844534</v>
       </c>
       <c r="Q14" s="23"/>
@@ -13522,7 +13660,7 @@
         <v>IT0003246292</v>
       </c>
       <c r="P15" s="48" t="str">
-        <f>_xll.qlBondMaturityLookup("StrippableBTPs",$H15,BTP!$I$96)</f>
+        <f>_xll.qlBondMaturityLookup("StrippableBTPs",$H15,BTP!$I$99)</f>
         <v>IT0004019581</v>
       </c>
       <c r="Q15" s="23"/>
@@ -13573,7 +13711,7 @@
         <v>IT0003246284</v>
       </c>
       <c r="P16" s="48" t="str">
-        <f>_xll.qlBondMaturityLookup("StrippableBTPs",$H16,BTP!$I$96)</f>
+        <f>_xll.qlBondMaturityLookup("StrippableBTPs",$H16,BTP!$I$99)</f>
         <v>IT0004164775</v>
       </c>
       <c r="Q16" s="23"/>
@@ -13624,7 +13762,7 @@
         <v>IT0003246268</v>
       </c>
       <c r="P17" s="48" t="str">
-        <f>_xll.qlBondMaturityLookup("StrippableBTPs",$H17,BTP!$I$96)</f>
+        <f>_xll.qlBondMaturityLookup("StrippableBTPs",$H17,BTP!$I$99)</f>
         <v>IT0003242747</v>
       </c>
       <c r="Q17" s="23"/>
@@ -13675,7 +13813,7 @@
         <v>IT0003268486</v>
       </c>
       <c r="P18" s="48" t="str">
-        <f>_xll.qlBondMaturityLookup("StrippableBTPs",$H18,BTP!$I$96)</f>
+        <f>_xll.qlBondMaturityLookup("StrippableBTPs",$H18,BTP!$I$99)</f>
         <v>IT0004273493</v>
       </c>
       <c r="Q18" s="23"/>
@@ -13726,7 +13864,7 @@
         <v>IT0003268494</v>
       </c>
       <c r="P19" s="48" t="str">
-        <f>_xll.qlBondMaturityLookup("StrippableBTPs",$H19,BTP!$I$96)</f>
+        <f>_xll.qlBondMaturityLookup("StrippableBTPs",$H19,BTP!$I$99)</f>
         <v>IT0004361041</v>
       </c>
       <c r="Q19" s="23"/>
@@ -13777,7 +13915,7 @@
         <v>IT0003268544</v>
       </c>
       <c r="P20" s="48" t="str">
-        <f>_xll.qlBondMaturityLookup("StrippableBTPs",$H20,BTP!$I$96)</f>
+        <f>_xll.qlBondMaturityLookup("StrippableBTPs",$H20,BTP!$I$99)</f>
         <v>IT0003493258</v>
       </c>
       <c r="Q20" s="23"/>
@@ -13828,7 +13966,7 @@
         <v>IT0003268601</v>
       </c>
       <c r="P21" s="48" t="str">
-        <f>_xll.qlBondMaturityLookup("StrippableBTPs",$H21,BTP!$I$96)</f>
+        <f>_xll.qlBondMaturityLookup("StrippableBTPs",$H21,BTP!$I$99)</f>
         <v>IT0003644769</v>
       </c>
       <c r="Q21" s="23"/>
@@ -13879,7 +14017,7 @@
         <v>IT0003268700</v>
       </c>
       <c r="P22" s="48" t="str">
-        <f>_xll.qlBondMaturityLookup("StrippableBTPs",$H22,BTP!$I$96)</f>
+        <f>_xll.qlBondMaturityLookup("StrippableBTPs",$H22,BTP!$I$99)</f>
         <v>IT0004009673</v>
       </c>
       <c r="Q22" s="23"/>
@@ -13930,7 +14068,7 @@
         <v>IT0003268791</v>
       </c>
       <c r="P23" s="48" t="str">
-        <f>_xll.qlBondMaturityLookup("StrippableBTPs",$H23,BTP!$I$96)</f>
+        <f>_xll.qlBondMaturityLookup("StrippableBTPs",$H23,BTP!$I$99)</f>
         <v>IT0004356843</v>
       </c>
       <c r="Q23" s="23"/>
@@ -13981,7 +14119,7 @@
         <v>IT0003269062</v>
       </c>
       <c r="P24" s="48" t="str">
-        <f>_xll.qlBondMaturityLookup("StrippableBTPs",$H24,BTP!$I$96)</f>
+        <f>_xll.qlBondMaturityLookup("StrippableBTPs",$H24,BTP!$I$99)</f>
         <v>IT0003256820</v>
       </c>
       <c r="Q24" s="23"/>
@@ -14032,7 +14170,7 @@
         <v>IT0003540405</v>
       </c>
       <c r="P25" s="48" t="str">
-        <f>_xll.qlBondMaturityLookup("StrippableBTPs",$H25,BTP!$I$96)</f>
+        <f>_xll.qlBondMaturityLookup("StrippableBTPs",$H25,BTP!$I$99)</f>
         <v>IT0003535157</v>
       </c>
       <c r="Q25" s="23"/>
@@ -14083,7 +14221,7 @@
         <v>IT0004002850</v>
       </c>
       <c r="P26" s="48" t="str">
-        <f>_xll.qlBondMaturityLookup("StrippableBTPs",$H26,BTP!$I$96)</f>
+        <f>_xll.qlBondMaturityLookup("StrippableBTPs",$H26,BTP!$I$99)</f>
         <v>IT0003934657</v>
       </c>
       <c r="Q26" s="23"/>
@@ -14134,7 +14272,7 @@
         <v>IT0004288640</v>
       </c>
       <c r="P27" s="48" t="str">
-        <f>_xll.qlBondMaturityLookup("StrippableBTPs",$H27,BTP!$I$96)</f>
+        <f>_xll.qlBondMaturityLookup("StrippableBTPs",$H27,BTP!$I$99)</f>
         <v>IT0004286966</v>
       </c>
       <c r="Q27" s="23"/>
@@ -17155,7 +17293,7 @@
         <v>IT0001247060</v>
       </c>
       <c r="P8" s="48" t="str">
-        <f>_xll.qlBondMaturityLookup(BTP!$I$96,$H8)</f>
+        <f>_xll.qlBondMaturityLookup(BTP!$I$99,$H8)</f>
         <v>IT0001448619</v>
       </c>
       <c r="Q8" s="23"/>
@@ -17206,7 +17344,7 @@
         <v>IT0001247326</v>
       </c>
       <c r="P9" s="48" t="str">
-        <f>_xll.qlBondMaturityLookup(BTP!$I$96,$H9)</f>
+        <f>_xll.qlBondMaturityLookup(BTP!$I$99,$H9)</f>
         <v>IT0000366655</v>
       </c>
       <c r="Q9" s="23"/>
@@ -17257,7 +17395,7 @@
         <v>IT0001247383</v>
       </c>
       <c r="P10" s="48" t="str">
-        <f>_xll.qlBondMaturityLookup(BTP!$I$96,$H10)</f>
+        <f>_xll.qlBondMaturityLookup(BTP!$I$99,$H10)</f>
         <v>IT0001086567</v>
       </c>
       <c r="Q10" s="23"/>
@@ -17308,7 +17446,7 @@
         <v>IT0001247409</v>
       </c>
       <c r="P11" s="48" t="str">
-        <f>_xll.qlBondMaturityLookup(BTP!$I$96,$H11)</f>
+        <f>_xll.qlBondMaturityLookup(BTP!$I$99,$H11)</f>
         <v>IT0001174611</v>
       </c>
       <c r="Q11" s="23"/>
@@ -17359,7 +17497,7 @@
         <v>IT0001312815</v>
       </c>
       <c r="P12" s="48" t="str">
-        <f>_xll.qlBondMaturityLookup(BTP!$I$96,$H12)</f>
+        <f>_xll.qlBondMaturityLookup(BTP!$I$99,$H12)</f>
         <v>IT0001278511</v>
       </c>
       <c r="Q12" s="23"/>
@@ -17410,7 +17548,7 @@
         <v>IT0001464210</v>
       </c>
       <c r="P13" s="48" t="str">
-        <f>_xll.qlBondMaturityLookup(BTP!$I$96,$H13)</f>
+        <f>_xll.qlBondMaturityLookup(BTP!$I$99,$H13)</f>
         <v>IT0001444378</v>
       </c>
       <c r="Q13" s="23"/>

</xml_diff>